<commit_message>
Add questions and answers to xlsx via cli
</commit_message>
<xml_diff>
--- a/faqs.xlsx
+++ b/faqs.xlsx
@@ -424,24 +424,24 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>q1</t>
+          <t>Is Cyber harassment also a Cybercrime ?</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>a1</t>
+          <t>Cyber harassment is a distinct Cybercrime. Various kinds of harassment can and does occur in cyberspace, or through the use of cyberspace. Harassment can be sexual, racial, religious, or other. Persons perpetuating such harassment are also guilty of cybercrimes. Cyber harassment as a crime also brings us to another related area of violation of privacy of netizens. Violation of privacy of online citizens is a Cybercrime of a grave nature. No one likes any other person invading the precious and extremely touchy area of his or her own privacy which the medium of Internet grants to the netizen.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>q2</t>
+          <t>n</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a2</t>
+          <t>test</t>
         </is>
       </c>
     </row>

</xml_diff>